<commit_message>
Adding Excel Map (Work in progress)
</commit_message>
<xml_diff>
--- a/docs/images/original_regions/Habitat_Region_Status.xlsx
+++ b/docs/images/original_regions/Habitat_Region_Status.xlsx
@@ -7,9 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Back 40" sheetId="2" r:id="rId2"/>
+    <sheet name="PopUStop" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,6 +148,55 @@
         </r>
       </text>
     </comment>
+    <comment ref="L18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Needs Oracle Class</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Need's Vendroid Class
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M24" authorId="0" shapeId="0">
       <text>
         <r>
@@ -176,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t xml:space="preserve">The Oracle
 </t>
@@ -312,13 +363,19 @@
   </si>
   <si>
     <t>Blocked (Hover for reason)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classes Needed: Oracle, Teleport, Vendroid, </t>
+  </si>
+  <si>
+    <t>Builders: @Steve, @Stuart, @neoedo1819(Matt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,14 +400,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -362,6 +411,21 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -515,86 +579,86 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -879,36 +943,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="1"/>
-    <col min="2" max="15" width="11.578125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="8.83984375" style="14"/>
+    <col min="2" max="12" width="11.578125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="13.89453125" style="14" customWidth="1"/>
+    <col min="14" max="15" width="11.578125" style="14" customWidth="1"/>
+    <col min="16" max="16384" width="8.83984375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="11"/>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
@@ -924,45 +992,50 @@
     </row>
     <row r="2" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="16" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
     </row>
     <row r="3" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="4" t="str">
+        <f>"+"</f>
+        <v>+</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="16" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
@@ -978,16 +1051,16 @@
     </row>
     <row r="4" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="16" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
@@ -1002,127 +1075,79 @@
       <c r="V4" s="26"/>
     </row>
     <row r="5" spans="2:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-    </row>
-    <row r="7" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="7" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="O7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="P7" s="18"/>
-    </row>
-    <row r="8" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+    </row>
+    <row r="8" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="M8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="18"/>
-    </row>
-    <row r="9" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="24" t="s">
+    </row>
+    <row r="9" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="25" t="s">
+      <c r="O9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="18"/>
-    </row>
-    <row r="10" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+    </row>
+    <row r="10" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="L10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-    </row>
-    <row r="11" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="21" t="s">
         <v>28</v>
       </c>
@@ -1156,12 +1181,8 @@
       <c r="L11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-    </row>
-    <row r="12" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="21" t="s">
         <v>29</v>
       </c>
@@ -1177,22 +1198,8 @@
       <c r="F12" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-    </row>
-    <row r="13" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+    </row>
+    <row r="13" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" s="21" t="s">
         <v>31</v>
       </c>
@@ -1214,163 +1221,93 @@
       <c r="L13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-    </row>
-    <row r="14" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="17" t="s">
+    </row>
+    <row r="14" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-    </row>
-    <row r="15" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="17" t="s">
+    </row>
+    <row r="15" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M15" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-    </row>
-    <row r="16" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="17" t="s">
+    </row>
+    <row r="16" spans="2:22" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M16" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-    </row>
-    <row r="17" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="17" t="s">
+    </row>
+    <row r="17" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-    </row>
-    <row r="18" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="17" t="s">
+    </row>
+    <row r="18" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="K18" s="21" t="s">
         <v>38</v>
       </c>
       <c r="L18" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="17" t="s">
+      <c r="M18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-    </row>
-    <row r="19" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M19" s="23" t="s">
+    </row>
+    <row r="19" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M19" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M20" s="17" t="s">
+    <row r="20" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M20" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M21" s="17" t="s">
+    <row r="21" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M22" s="17" t="s">
+    <row r="22" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M22" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M23" s="17" t="s">
+    <row r="23" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M23" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M24" s="17" t="s">
+    <row r="24" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="M24" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="11:14" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="J1:V1"/>
     <mergeCell ref="J2:V2"/>
     <mergeCell ref="J3:V3"/>
     <mergeCell ref="J4:V4"/>
     <mergeCell ref="J5:V5"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N8" r:id="rId1" display="Plaza_Center-Oracle.JPG"/>
+    <hyperlink ref="N8" r:id="rId1" display="https://github.com/frandallfarmer/neohabitat/tree/master/docs/images/original_regions/Plaza_Center-Oracle.JPG"/>
     <hyperlink ref="M8" r:id="rId2"/>
     <hyperlink ref="M9" r:id="rId3"/>
     <hyperlink ref="M10" r:id="rId4"/>
@@ -1418,4 +1355,28 @@
   <pageSetup orientation="portrait" r:id="rId44"/>
   <legacyDrawing r:id="rId45"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>